<commit_message>
results: calculate "Tomita" condition
</commit_message>
<xml_diff>
--- a/result_summary.xlsx
+++ b/result_summary.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/152b4070cb6fc60a/programs/Research/Physical_calculation/Kaneko_framework_drude_function/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/152b4070cb6fc60a/programs/Research/Physical_calculation/Cluster_stopping_calculation_drude_function/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="41" documentId="8_{B4C675F8-E733-415A-9DD8-47743EEB9A7A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{2FD2AC45-54A9-4AC2-9340-4125A13A914F}"/>
+  <xr:revisionPtr revIDLastSave="85" documentId="8_{B4C675F8-E733-415A-9DD8-47743EEB9A7A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{203E461E-1FE4-49D8-8BBF-84B01C8EE30A}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{865C7646-31E9-4D0E-827F-A9F4C02E8C84}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{865C7646-31E9-4D0E-827F-A9F4C02E8C84}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="single_velocity_dependence" sheetId="1" r:id="rId1"/>
+    <sheet name="orientation_averaged_size_dep" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Ec(keV/atom)</t>
     <phoneticPr fontId="1"/>
@@ -53,6 +54,18 @@
   </si>
   <si>
     <t>SRIM</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>500keV/atom</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>n</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Se (eV/A) of Gly myCalc</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -150,7 +163,7 @@
           </c:spPr>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$B$3:$B$9</c:f>
+              <c:f>single_velocity_dependence!$B$4:$B$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -180,7 +193,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$D$3:$D$9</c:f>
+              <c:f>single_velocity_dependence!$D$4:$D$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -242,29 +255,32 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$B$3:$B$9</c:f>
+              <c:f>single_velocity_dependence!$B$3:$B$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>800</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>900</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>1000</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>1200</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>1400</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>1600</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>1800</c:v>
                 </c:pt>
               </c:numCache>
@@ -272,29 +288,32 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$3:$C$9</c:f>
+              <c:f>single_velocity_dependence!$C$3:$C$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
+                  <c:v>13.692363590644099</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>46.964787119721898</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>54.935931799608298</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>61.414845913487298</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>71.141020930611305</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>77.948407203899905</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>82.861866739268805</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>86.486080240866997</c:v>
                 </c:pt>
               </c:numCache>
@@ -470,16 +489,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>312420</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>99060</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>144780</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>91440</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>102870</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>182880</xdr:rowOff>
+      <xdr:colOff>605790</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>175260</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -804,10 +823,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FEE0BAA-93F5-4CBD-8DE0-95F353D45A6C}">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q14" sqref="Q14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.45"/>
@@ -833,78 +852,86 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B3">
-        <v>800</v>
+        <v>500</v>
       </c>
       <c r="C3">
-        <v>46.964787119721898</v>
-      </c>
-      <c r="D3">
-        <v>52.73</v>
+        <v>13.692363590644099</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B4">
-        <v>900</v>
+        <v>800</v>
       </c>
       <c r="C4">
-        <v>54.935931799608298</v>
+        <v>46.964787119721898</v>
       </c>
       <c r="D4">
-        <v>56.18</v>
+        <v>52.73</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B5">
-        <v>1000</v>
+        <v>900</v>
       </c>
       <c r="C5">
-        <v>61.414845913487298</v>
+        <v>54.935931799608298</v>
       </c>
       <c r="D5">
-        <v>59.45</v>
+        <v>56.18</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B6">
-        <v>1200</v>
+        <v>1000</v>
       </c>
       <c r="C6">
-        <v>71.141020930611305</v>
+        <v>61.414845913487298</v>
       </c>
       <c r="D6">
-        <v>65.52</v>
+        <v>59.45</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B7">
-        <v>1400</v>
+        <v>1200</v>
       </c>
       <c r="C7">
-        <v>77.948407203899905</v>
+        <v>71.141020930611305</v>
       </c>
       <c r="D7">
-        <v>70.95</v>
+        <v>65.52</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B8">
-        <v>1600</v>
+        <v>1400</v>
       </c>
       <c r="C8">
-        <v>82.861866739268805</v>
+        <v>77.948407203899905</v>
       </c>
       <c r="D8">
-        <v>75.739999999999995</v>
+        <v>70.95</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B9">
+        <v>1600</v>
+      </c>
+      <c r="C9">
+        <v>82.861866739268805</v>
+      </c>
+      <c r="D9">
+        <v>75.739999999999995</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B10">
         <v>1800</v>
       </c>
-      <c r="C9">
+      <c r="C10">
         <v>86.486080240866997</v>
       </c>
-      <c r="D9">
+      <c r="D10">
         <v>79.91</v>
       </c>
     </row>
@@ -914,4 +941,81 @@
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53858F9E-6685-4AD6-BA2B-9115073A2CE8}">
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.45"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>13.692363590644099</v>
+      </c>
+      <c r="C3">
+        <f>B3/A3-$B$3</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>29.165757927828398</v>
+      </c>
+      <c r="C4">
+        <f>B4/A4-$B$3</f>
+        <v>0.89051537327009989</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>43.221499705741302</v>
+      </c>
+      <c r="C5">
+        <f>B5/A5-$B$3</f>
+        <v>0.71480297793633518</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>55.883402139366503</v>
+      </c>
+      <c r="C6">
+        <f>B6/A6-$B$3</f>
+        <v>0.2784869441975264</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
update: brush up graph
</commit_message>
<xml_diff>
--- a/result_summary.xlsx
+++ b/result_summary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/152b4070cb6fc60a/programs/Research/Physical_calculation/Cluster_stopping_calculation_drude_function/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="85" documentId="8_{B4C675F8-E733-415A-9DD8-47743EEB9A7A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{203E461E-1FE4-49D8-8BBF-84B01C8EE30A}"/>
+  <xr:revisionPtr revIDLastSave="107" documentId="8_{B4C675F8-E733-415A-9DD8-47743EEB9A7A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{C0DEB4B2-D972-4359-9320-3F2D8C6F0DE0}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{865C7646-31E9-4D0E-827F-A9F4C02E8C84}"/>
   </bookViews>
@@ -156,6 +156,17 @@
         <c:ser>
           <c:idx val="1"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>single_velocity_dependence!$D$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>SRIM</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
           <c:spPr>
             <a:ln w="19050">
               <a:noFill/>
@@ -163,29 +174,32 @@
           </c:spPr>
           <c:xVal>
             <c:numRef>
-              <c:f>single_velocity_dependence!$B$4:$B$10</c:f>
+              <c:f>single_velocity_dependence!$B$3:$B$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>800</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>900</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>1000</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>1200</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>1400</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>1600</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>1800</c:v>
                 </c:pt>
               </c:numCache>
@@ -193,29 +207,32 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>single_velocity_dependence!$D$4:$D$10</c:f>
+              <c:f>single_velocity_dependence!$D$3:$D$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
+                  <c:v>41.19</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>52.73</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>56.18</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>59.45</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>65.52</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>70.95</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>75.739999999999995</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>79.91</c:v>
                 </c:pt>
               </c:numCache>
@@ -231,6 +248,17 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>single_velocity_dependence!$C$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>myCalc</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:noFill/>
@@ -462,6 +490,20 @@
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.19533035419131034"/>
+          <c:y val="0.12196736277530526"/>
+          <c:w val="0.1167035076609354"/>
+          <c:h val="0.13103560424512153"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="1"/>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -485,20 +527,895 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="ja-JP"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="ja-JP"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>orientation_averaged_size_dep!$C$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>orientation_averaged_size_dep!$A$3:$A$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>orientation_averaged_size_dep!$C$3:$C$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.89051537327009989</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.71480297793633518</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.2784869441975264</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-D5BF-4C01-939A-7C5C446CBC4F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="86730176"/>
+        <c:axId val="86766784"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="86730176"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ja-JP"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="86766784"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="86766784"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ja-JP"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="86730176"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="ja-JP"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>144780</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>91440</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>83820</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>60960</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>605790</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>175260</xdr:rowOff>
+      <xdr:colOff>411480</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>137160</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -506,6 +1423,47 @@
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3433E864-708C-4B92-B1D9-1BD7EE0C6462}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>339090</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>160020</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>217170</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>160020</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="グラフ 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AED0588B-C67E-4326-9DA0-3879292E3A98}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -826,7 +1784,7 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.45"/>
@@ -856,6 +1814,9 @@
       </c>
       <c r="C3">
         <v>13.692363590644099</v>
+      </c>
+      <c r="D3">
+        <v>41.19</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.45">
@@ -948,7 +1909,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.45"/>
@@ -1017,5 +1978,7 @@
   </sheetData>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
results: calculated for single ions in lower velo
</commit_message>
<xml_diff>
--- a/result_summary.xlsx
+++ b/result_summary.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/152b4070cb6fc60a/programs/Research/Physical_calculation/Cluster_stopping_calculation_drude_function/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="107" documentId="8_{B4C675F8-E733-415A-9DD8-47743EEB9A7A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{C0DEB4B2-D972-4359-9320-3F2D8C6F0DE0}"/>
+  <xr:revisionPtr revIDLastSave="165" documentId="8_{B4C675F8-E733-415A-9DD8-47743EEB9A7A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{74462A4B-0376-4B0A-A4DD-48AB46A87EAA}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{865C7646-31E9-4D0E-827F-A9F4C02E8C84}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{865C7646-31E9-4D0E-827F-A9F4C02E8C84}"/>
   </bookViews>
   <sheets>
     <sheet name="single_velocity_dependence" sheetId="1" r:id="rId1"/>
     <sheet name="orientation_averaged_size_dep" sheetId="2" r:id="rId2"/>
+    <sheet name="dimer_orientation_velocity_dep" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
   <si>
     <t>Ec(keV/atom)</t>
     <phoneticPr fontId="1"/>
@@ -66,6 +67,14 @@
   </si>
   <si>
     <t>Se (eV/A) of Gly myCalc</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>parallel(0-30deg)</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>perpendicular(60-90deg)</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -112,8 +121,11 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -174,32 +186,44 @@
           </c:spPr>
           <c:xVal>
             <c:numRef>
-              <c:f>single_velocity_dependence!$B$3:$B$10</c:f>
+              <c:f>single_velocity_dependence!$B$3:$B$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>500</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="5">
                   <c:v>800</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="6">
                   <c:v>900</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="7">
                   <c:v>1000</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="8">
                   <c:v>1200</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="9">
                   <c:v>1400</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="10">
                   <c:v>1600</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="11">
                   <c:v>1800</c:v>
                 </c:pt>
               </c:numCache>
@@ -207,32 +231,44 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>single_velocity_dependence!$D$3:$D$10</c:f>
+              <c:f>single_velocity_dependence!$D$3:$D$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
+                  <c:v>2.2130000000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>19.690000000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>29.24</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>41.19</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="5">
                   <c:v>52.73</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="6">
                   <c:v>56.18</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="7">
                   <c:v>59.45</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="8">
                   <c:v>65.52</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="9">
                   <c:v>70.95</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="10">
                   <c:v>75.739999999999995</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="11">
                   <c:v>79.91</c:v>
                 </c:pt>
               </c:numCache>
@@ -283,32 +319,44 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>single_velocity_dependence!$B$3:$B$10</c:f>
+              <c:f>single_velocity_dependence!$B$3:$B$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>500</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="5">
                   <c:v>800</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="6">
                   <c:v>900</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="7">
                   <c:v>1000</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="8">
                   <c:v>1200</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="9">
                   <c:v>1400</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="10">
                   <c:v>1600</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="11">
                   <c:v>1800</c:v>
                 </c:pt>
               </c:numCache>
@@ -316,32 +364,44 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>single_velocity_dependence!$C$3:$C$10</c:f>
+              <c:f>single_velocity_dependence!$C$3:$C$14</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
+                  <c:v>3.9725393728110001E-8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.3302344856923799E-5</c:v>
+                </c:pt>
+                <c:pt idx="2" formatCode="General">
+                  <c:v>5.3112578690337003E-2</c:v>
+                </c:pt>
+                <c:pt idx="3" formatCode="General">
+                  <c:v>1.02597388458987</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="General">
                   <c:v>13.692363590644099</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="5" formatCode="General">
                   <c:v>46.964787119721898</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="6" formatCode="General">
                   <c:v>54.935931799608298</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="7" formatCode="General">
                   <c:v>61.414845913487298</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="8" formatCode="General">
                   <c:v>71.141020930611305</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="9" formatCode="General">
                   <c:v>77.948407203899905</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="10" formatCode="General">
                   <c:v>82.861866739268805</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="11" formatCode="General">
                   <c:v>86.486080240866997</c:v>
                 </c:pt>
               </c:numCache>
@@ -846,7 +906,489 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="ja-JP"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>dimer_orientation_velocity_dep!$B$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>parallel(0-30deg)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>dimer_orientation_velocity_dep!$A$3:$A$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>800</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1200</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1400</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1600</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1800</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>dimer_orientation_velocity_dep!$B$3:$B$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>65.265169335175301</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>102.38953918855699</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>126.652990240788</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>140.38543969933801</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>148.97984903241201</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>156.32886358168099</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-B18A-47A7-9B23-7A3B6BA66FFB}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>dimer_orientation_velocity_dep!$C$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>perpendicular(60-90deg)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>dimer_orientation_velocity_dep!$A$3:$A$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>800</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1200</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1400</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1600</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1800</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>dimer_orientation_velocity_dep!$C$3:$C$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>111.073779304095</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>135.94792750511201</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>152.46881312489899</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>165.04462065710399</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>174.98739252174499</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>182.74128622324301</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-B18A-47A7-9B23-7A3B6BA66FFB}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1836113824"/>
+        <c:axId val="1836109248"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1836113824"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ja-JP"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1836109248"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1836109248"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ja-JP"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1836113824"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.10882296186626646"/>
+          <c:y val="8.848270370698047E-2"/>
+          <c:w val="0.30488090186331501"/>
+          <c:h val="0.11867171666832786"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="1"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="ja-JP"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="ja-JP"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -1402,20 +1944,536 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>83820</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>60960</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>274320</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>144780</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>411480</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>137160</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>601980</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>220980</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1464,6 +2522,47 @@
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AED0588B-C67E-4326-9DA0-3879292E3A98}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>217170</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>175260</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>647700</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>129540</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="グラフ 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F75185CE-F739-480E-B910-396648217355}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1781,10 +2880,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FEE0BAA-93F5-4CBD-8DE0-95F353D45A6C}">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.45"/>
@@ -1810,89 +2909,133 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B3">
-        <v>500</v>
-      </c>
-      <c r="C3">
-        <v>13.692363590644099</v>
+        <v>1</v>
+      </c>
+      <c r="C3" s="1">
+        <v>3.9725393728110001E-8</v>
       </c>
       <c r="D3">
-        <v>41.19</v>
+        <v>2.2130000000000001</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B4">
-        <v>800</v>
-      </c>
-      <c r="C4">
-        <v>46.964787119721898</v>
+        <v>10</v>
+      </c>
+      <c r="C4" s="1">
+        <v>4.3302344856923799E-5</v>
       </c>
       <c r="D4">
-        <v>52.73</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B5">
-        <v>900</v>
+        <v>100</v>
       </c>
       <c r="C5">
-        <v>54.935931799608298</v>
+        <v>5.3112578690337003E-2</v>
       </c>
       <c r="D5">
-        <v>56.18</v>
+        <v>19.690000000000001</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B6">
-        <v>1000</v>
+        <v>250</v>
       </c>
       <c r="C6">
-        <v>61.414845913487298</v>
+        <v>1.02597388458987</v>
       </c>
       <c r="D6">
-        <v>59.45</v>
+        <v>29.24</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B7">
-        <v>1200</v>
+        <v>500</v>
       </c>
       <c r="C7">
-        <v>71.141020930611305</v>
+        <v>13.692363590644099</v>
       </c>
       <c r="D7">
-        <v>65.52</v>
+        <v>41.19</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B8">
-        <v>1400</v>
+        <v>800</v>
       </c>
       <c r="C8">
-        <v>77.948407203899905</v>
+        <v>46.964787119721898</v>
       </c>
       <c r="D8">
-        <v>70.95</v>
+        <v>52.73</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B9">
-        <v>1600</v>
+        <v>900</v>
       </c>
       <c r="C9">
-        <v>82.861866739268805</v>
+        <v>54.935931799608298</v>
       </c>
       <c r="D9">
-        <v>75.739999999999995</v>
+        <v>56.18</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B10">
+        <v>1000</v>
+      </c>
+      <c r="C10">
+        <v>61.414845913487298</v>
+      </c>
+      <c r="D10">
+        <v>59.45</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B11">
+        <v>1200</v>
+      </c>
+      <c r="C11">
+        <v>71.141020930611305</v>
+      </c>
+      <c r="D11">
+        <v>65.52</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B12">
+        <v>1400</v>
+      </c>
+      <c r="C12">
+        <v>77.948407203899905</v>
+      </c>
+      <c r="D12">
+        <v>70.95</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B13">
+        <v>1600</v>
+      </c>
+      <c r="C13">
+        <v>82.861866739268805</v>
+      </c>
+      <c r="D13">
+        <v>75.739999999999995</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B14">
         <v>1800</v>
       </c>
-      <c r="C10">
+      <c r="C14">
         <v>86.486080240866997</v>
       </c>
-      <c r="D10">
+      <c r="D14">
         <v>79.91</v>
       </c>
     </row>
@@ -1908,8 +3051,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53858F9E-6685-4AD6-BA2B-9115073A2CE8}">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.45"/>
@@ -1973,6 +3116,109 @@
       <c r="C6">
         <f>B6/A6-$B$3</f>
         <v>0.2784869441975264</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D4C90C0-5DE0-45E3-A223-4CC7D5EF3006}">
+  <dimension ref="A1:C8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M16" sqref="M16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="2" max="3" width="16.8984375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A3">
+        <v>800</v>
+      </c>
+      <c r="B3">
+        <v>65.265169335175301</v>
+      </c>
+      <c r="C3">
+        <v>111.073779304095</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A4">
+        <v>1000</v>
+      </c>
+      <c r="B4">
+        <v>102.38953918855699</v>
+      </c>
+      <c r="C4">
+        <v>135.94792750511201</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A5">
+        <v>1200</v>
+      </c>
+      <c r="B5">
+        <v>126.652990240788</v>
+      </c>
+      <c r="C5">
+        <v>152.46881312489899</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A6">
+        <v>1400</v>
+      </c>
+      <c r="B6">
+        <v>140.38543969933801</v>
+      </c>
+      <c r="C6">
+        <v>165.04462065710399</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A7">
+        <v>1600</v>
+      </c>
+      <c r="B7">
+        <v>148.97984903241201</v>
+      </c>
+      <c r="C7">
+        <v>174.98739252174499</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A8">
+        <v>1800</v>
+      </c>
+      <c r="B8">
+        <v>156.32886358168099</v>
+      </c>
+      <c r="C8">
+        <v>182.74128622324301</v>
       </c>
     </row>
   </sheetData>

</xml_diff>